<commit_message>
version 3 of the generated data. Two signals were still missing - added on request from Rein
git-svn-id: https://biosemantics.org/svn/EUADR@5579 73ab80c8-c28e-48d9-a4b9-bb1e898e81ef
</commit_message>
<xml_diff>
--- a/data/negative_signals/Disease - Total occurrences (B-to-X) - Tiotropium bromide - all categories.xlsx
+++ b/data/negative_signals/Disease - Total occurrences (B-to-X) - Tiotropium bromide - all categories.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="331">
   <si>
     <t>pathWeight</t>
   </si>
@@ -102,31 +102,181 @@
     <t>Chemicals &amp; Drugs</t>
   </si>
   <si>
-    <t>3780811</t>
-  </si>
-  <si>
-    <t>ba 679 br</t>
-  </si>
-  <si>
-    <t>159506550</t>
+    <t>3244307</t>
+  </si>
+  <si>
+    <t>tiotropium bromide</t>
+  </si>
+  <si>
+    <t>89903399</t>
+  </si>
+  <si>
+    <t>coexists with</t>
+  </si>
+  <si>
+    <t>64510312</t>
   </si>
   <si>
     <t>is a</t>
   </si>
   <si>
+    <t>116913534</t>
+  </si>
+  <si>
+    <t>interacts with</t>
+  </si>
+  <si>
+    <t>836626</t>
+  </si>
+  <si>
+    <t>sodium chloride</t>
+  </si>
+  <si>
+    <t>100780392</t>
+  </si>
+  <si>
+    <t>308092</t>
+  </si>
+  <si>
+    <t>agonists</t>
+  </si>
+  <si>
+    <t>59550944</t>
+  </si>
+  <si>
+    <t>is compared with</t>
+  </si>
+  <si>
+    <t>2723200</t>
+  </si>
+  <si>
+    <t>peroxisome proliferator-activated receptor gamma (homo sapiens)</t>
+  </si>
+  <si>
+    <t>124654214</t>
+  </si>
+  <si>
+    <t>stimulates</t>
+  </si>
+  <si>
+    <t>4832001</t>
+  </si>
+  <si>
+    <t>adrenal cortex hormones</t>
+  </si>
+  <si>
+    <t>129810777</t>
+  </si>
+  <si>
+    <t>332232</t>
+  </si>
+  <si>
+    <t>transforming growth factor beta-1 (homo sapiens)</t>
+  </si>
+  <si>
+    <t>82827477</t>
+  </si>
+  <si>
+    <t>inhibits</t>
+  </si>
+  <si>
+    <t>3097558</t>
+  </si>
+  <si>
+    <t>human plasma</t>
+  </si>
+  <si>
+    <t>132639009</t>
+  </si>
+  <si>
+    <t>5797677</t>
+  </si>
+  <si>
+    <t>interleukin-8</t>
+  </si>
+  <si>
+    <t>52909661</t>
+  </si>
+  <si>
+    <t>does not interact with</t>
+  </si>
+  <si>
+    <t>75901957</t>
+  </si>
+  <si>
+    <t>4042246</t>
+  </si>
+  <si>
+    <t>atropine</t>
+  </si>
+  <si>
+    <t>64311605</t>
+  </si>
+  <si>
+    <t>4608741</t>
+  </si>
+  <si>
+    <t>muscarinic acetylcholine receptor</t>
+  </si>
+  <si>
+    <t>82820304</t>
+  </si>
+  <si>
+    <t>169684</t>
+  </si>
+  <si>
+    <t>albuterol</t>
+  </si>
+  <si>
+    <t>74604333</t>
+  </si>
+  <si>
+    <t>787076</t>
+  </si>
+  <si>
+    <t>mitogen activated protein kinase 1</t>
+  </si>
+  <si>
+    <t>110331952</t>
+  </si>
+  <si>
+    <t>4042156</t>
+  </si>
+  <si>
+    <t>bromides</t>
+  </si>
+  <si>
+    <t>127384283</t>
+  </si>
+  <si>
+    <t>752437</t>
+  </si>
+  <si>
+    <t>budesonide</t>
+  </si>
+  <si>
+    <t>126641698</t>
+  </si>
+  <si>
     <t>425645</t>
   </si>
   <si>
     <t>anticholinergic agents</t>
   </si>
   <si>
-    <t>159505872</t>
-  </si>
-  <si>
-    <t>interacts with</t>
-  </si>
-  <si>
-    <t>159505796</t>
+    <t>61085797</t>
+  </si>
+  <si>
+    <t>110759721</t>
+  </si>
+  <si>
+    <t>2735484</t>
+  </si>
+  <si>
+    <t>beta-2</t>
+  </si>
+  <si>
+    <t>124011562</t>
   </si>
   <si>
     <t>834030</t>
@@ -135,22 +285,10 @@
     <t>muscarinic antagonists</t>
   </si>
   <si>
-    <t>130784319</t>
-  </si>
-  <si>
-    <t>159506044</t>
-  </si>
-  <si>
-    <t>4742521</t>
-  </si>
-  <si>
-    <t>oxotremorine</t>
-  </si>
-  <si>
-    <t>85333292</t>
-  </si>
-  <si>
-    <t>inhibits</t>
+    <t>108402106</t>
+  </si>
+  <si>
+    <t>59040176</t>
   </si>
   <si>
     <t>290243</t>
@@ -159,16 +297,22 @@
     <t>bronchodilator agents</t>
   </si>
   <si>
-    <t>143640711</t>
-  </si>
-  <si>
-    <t>3784382</t>
-  </si>
-  <si>
-    <t>receptor, muscarinic m3</t>
-  </si>
-  <si>
-    <t>159506484</t>
+    <t>107249384</t>
+  </si>
+  <si>
+    <t>114577539</t>
+  </si>
+  <si>
+    <t>90675614</t>
+  </si>
+  <si>
+    <t>532117</t>
+  </si>
+  <si>
+    <t>formoterol</t>
+  </si>
+  <si>
+    <t>103153503</t>
   </si>
   <si>
     <t>776533</t>
@@ -177,10 +321,34 @@
     <t>ipratropium bromide</t>
   </si>
   <si>
-    <t>153063239</t>
-  </si>
-  <si>
-    <t>is compared with</t>
+    <t>90154689</t>
+  </si>
+  <si>
+    <t>92354375</t>
+  </si>
+  <si>
+    <t>is higher than</t>
+  </si>
+  <si>
+    <t>710854</t>
+  </si>
+  <si>
+    <t>glycopyrrolate</t>
+  </si>
+  <si>
+    <t>82883031</t>
+  </si>
+  <si>
+    <t>3381154</t>
+  </si>
+  <si>
+    <t>desloratadine</t>
+  </si>
+  <si>
+    <t>68884076</t>
+  </si>
+  <si>
+    <t>68884172</t>
   </si>
   <si>
     <t>686821</t>
@@ -189,16 +357,112 @@
     <t>tiotropium</t>
   </si>
   <si>
-    <t>177428611</t>
-  </si>
-  <si>
-    <t>203587590</t>
+    <t>137402112</t>
   </si>
   <si>
     <t>is parent of</t>
   </si>
   <si>
-    <t>159505964</t>
+    <t>53785995</t>
+  </si>
+  <si>
+    <t>137402110</t>
+  </si>
+  <si>
+    <t>converts to</t>
+  </si>
+  <si>
+    <t>132980497</t>
+  </si>
+  <si>
+    <t>126641831</t>
+  </si>
+  <si>
+    <t>138834541</t>
+  </si>
+  <si>
+    <t>3200359</t>
+  </si>
+  <si>
+    <t>budesonide / formoterol</t>
+  </si>
+  <si>
+    <t>90558748</t>
+  </si>
+  <si>
+    <t>132515986</t>
+  </si>
+  <si>
+    <t>5206046</t>
+  </si>
+  <si>
+    <t>tulobuterol</t>
+  </si>
+  <si>
+    <t>89461699</t>
+  </si>
+  <si>
+    <t>89462460</t>
+  </si>
+  <si>
+    <t>108404151</t>
+  </si>
+  <si>
+    <t>632003</t>
+  </si>
+  <si>
+    <t>fluticasone / salmeterol</t>
+  </si>
+  <si>
+    <t>89231415</t>
+  </si>
+  <si>
+    <t>2708436</t>
+  </si>
+  <si>
+    <t>fluticasone propionate, salmeterol xinafoate drug combination</t>
+  </si>
+  <si>
+    <t>129814515</t>
+  </si>
+  <si>
+    <t>3051768</t>
+  </si>
+  <si>
+    <t>bronchodilators,anticholinergic</t>
+  </si>
+  <si>
+    <t>51416409</t>
+  </si>
+  <si>
+    <t>786855</t>
+  </si>
+  <si>
+    <t>spiriva</t>
+  </si>
+  <si>
+    <t>59998426</t>
+  </si>
+  <si>
+    <t>47573</t>
+  </si>
+  <si>
+    <t>cells</t>
+  </si>
+  <si>
+    <t>Anatomy</t>
+  </si>
+  <si>
+    <t>75973185</t>
+  </si>
+  <si>
+    <t>is location of</t>
+  </si>
+  <si>
+    <t>78386045</t>
+  </si>
+  <si>
+    <t>disrupts</t>
   </si>
   <si>
     <t>719023</t>
@@ -207,34 +471,94 @@
     <t>lung</t>
   </si>
   <si>
-    <t>Anatomy</t>
-  </si>
-  <si>
-    <t>153062989</t>
-  </si>
-  <si>
-    <t>is location of</t>
-  </si>
-  <si>
-    <t>836697</t>
-  </si>
-  <si>
-    <t>bronchi</t>
-  </si>
-  <si>
-    <t>159506619</t>
-  </si>
-  <si>
-    <t>2786189</t>
-  </si>
-  <si>
-    <t>edn1 (homo sapiens)</t>
+    <t>64311273</t>
+  </si>
+  <si>
+    <t>4035461</t>
+  </si>
+  <si>
+    <t>fibroblasts</t>
+  </si>
+  <si>
+    <t>75977803</t>
+  </si>
+  <si>
+    <t>116798012</t>
+  </si>
+  <si>
+    <t>4042029</t>
+  </si>
+  <si>
+    <t>epithelial cells</t>
+  </si>
+  <si>
+    <t>76004764</t>
+  </si>
+  <si>
+    <t>81553</t>
+  </si>
+  <si>
+    <t>macrophages, alveolar</t>
+  </si>
+  <si>
+    <t>52755449</t>
+  </si>
+  <si>
+    <t>3139102</t>
+  </si>
+  <si>
+    <t>inflammatory cells</t>
+  </si>
+  <si>
+    <t>100780417</t>
+  </si>
+  <si>
+    <t>102712</t>
+  </si>
+  <si>
+    <t>myofibroblasts</t>
+  </si>
+  <si>
+    <t>116797970</t>
+  </si>
+  <si>
+    <t>2398742</t>
+  </si>
+  <si>
+    <t>biological membrane</t>
+  </si>
+  <si>
+    <t>114220036</t>
+  </si>
+  <si>
+    <t>1658339</t>
+  </si>
+  <si>
+    <t>nfkb1 (homo sapiens)</t>
   </si>
   <si>
     <t>Genes &amp; Molecular Sequences</t>
   </si>
   <si>
-    <t>85333301</t>
+    <t>112836753</t>
+  </si>
+  <si>
+    <t>2474013</t>
+  </si>
+  <si>
+    <t>rhoa (homo sapiens)</t>
+  </si>
+  <si>
+    <t>88325364</t>
+  </si>
+  <si>
+    <t>2548226</t>
+  </si>
+  <si>
+    <t>mmp gene</t>
+  </si>
+  <si>
+    <t>97754728</t>
   </si>
   <si>
     <t>2792269</t>
@@ -243,7 +567,7 @@
     <t>chrm1 (homo sapiens)</t>
   </si>
   <si>
-    <t>115002046</t>
+    <t>48809860</t>
   </si>
   <si>
     <t>affects</t>
@@ -255,7 +579,7 @@
     <t>chrm3 (homo sapiens)</t>
   </si>
   <si>
-    <t>115002067</t>
+    <t>48809881</t>
   </si>
   <si>
     <t>3019735</t>
@@ -264,16 +588,94 @@
     <t>chrm2 (homo sapiens)</t>
   </si>
   <si>
-    <t>115002057</t>
-  </si>
-  <si>
-    <t>2767462</t>
-  </si>
-  <si>
-    <t>nms (homo sapiens)</t>
-  </si>
-  <si>
-    <t>153063400</t>
+    <t>48809871</t>
+  </si>
+  <si>
+    <t>837423</t>
+  </si>
+  <si>
+    <t>disease</t>
+  </si>
+  <si>
+    <t>Disorders</t>
+  </si>
+  <si>
+    <t>120751201</t>
+  </si>
+  <si>
+    <t>treats</t>
+  </si>
+  <si>
+    <t>5223016</t>
+  </si>
+  <si>
+    <t>syndrome</t>
+  </si>
+  <si>
+    <t>102708107</t>
+  </si>
+  <si>
+    <t>45119</t>
+  </si>
+  <si>
+    <t>inflammation</t>
+  </si>
+  <si>
+    <t>82841712</t>
+  </si>
+  <si>
+    <t>82820073</t>
+  </si>
+  <si>
+    <t>2940375</t>
+  </si>
+  <si>
+    <t>symptoms</t>
+  </si>
+  <si>
+    <t>108244622</t>
+  </si>
+  <si>
+    <t>3072277</t>
+  </si>
+  <si>
+    <t>antimicrobial susceptibility</t>
+  </si>
+  <si>
+    <t>103798212</t>
+  </si>
+  <si>
+    <t>3131611</t>
+  </si>
+  <si>
+    <t>observation parameter</t>
+  </si>
+  <si>
+    <t>100780361</t>
+  </si>
+  <si>
+    <t>2552993</t>
+  </si>
+  <si>
+    <t>cerebrovascular accident</t>
+  </si>
+  <si>
+    <t>109331623</t>
+  </si>
+  <si>
+    <t>predisposes</t>
+  </si>
+  <si>
+    <t>1595282</t>
+  </si>
+  <si>
+    <t>asthma</t>
+  </si>
+  <si>
+    <t>64312183</t>
+  </si>
+  <si>
+    <t>99279247</t>
   </si>
   <si>
     <t>3262699</t>
@@ -282,13 +684,16 @@
     <t>contraction (finding)</t>
   </si>
   <si>
-    <t>Disorders</t>
-  </si>
-  <si>
-    <t>159506245</t>
-  </si>
-  <si>
-    <t>disrupts</t>
+    <t>118118070</t>
+  </si>
+  <si>
+    <t>425414</t>
+  </si>
+  <si>
+    <t>tuberculosis</t>
+  </si>
+  <si>
+    <t>89555162</t>
   </si>
   <si>
     <t>881200</t>
@@ -297,25 +702,313 @@
     <t>chronic obstructive airway disease</t>
   </si>
   <si>
-    <t>143640810</t>
+    <t>125487462</t>
+  </si>
+  <si>
+    <t>prevents</t>
+  </si>
+  <si>
+    <t>53093008</t>
+  </si>
+  <si>
+    <t>584032</t>
+  </si>
+  <si>
+    <t>ulcer</t>
+  </si>
+  <si>
+    <t>109064171</t>
+  </si>
+  <si>
+    <t>causes</t>
+  </si>
+  <si>
+    <t>465111</t>
+  </si>
+  <si>
+    <t>lung diseases</t>
+  </si>
+  <si>
+    <t>96201479</t>
+  </si>
+  <si>
+    <t>507191</t>
+  </si>
+  <si>
+    <t>dyspnea</t>
+  </si>
+  <si>
+    <t>61089712</t>
+  </si>
+  <si>
+    <t>94878428</t>
+  </si>
+  <si>
+    <t>125486649</t>
+  </si>
+  <si>
+    <t>3110750</t>
+  </si>
+  <si>
+    <t>paralysed</t>
+  </si>
+  <si>
+    <t>86996772</t>
+  </si>
+  <si>
+    <t>5123922</t>
+  </si>
+  <si>
+    <t>tachyarrhythmia</t>
+  </si>
+  <si>
+    <t>73586015</t>
+  </si>
+  <si>
+    <t>4047799</t>
+  </si>
+  <si>
+    <t>chronic inflammation, nos</t>
+  </si>
+  <si>
+    <t>82820826</t>
+  </si>
+  <si>
+    <t>5204334</t>
+  </si>
+  <si>
+    <t>burn injury</t>
+  </si>
+  <si>
+    <t>110331838</t>
+  </si>
+  <si>
+    <t>825581</t>
+  </si>
+  <si>
+    <t>personal satisfaction</t>
+  </si>
+  <si>
+    <t>105636014</t>
+  </si>
+  <si>
+    <t>5796922</t>
+  </si>
+  <si>
+    <t>allergic asthma</t>
+  </si>
+  <si>
+    <t>61865227</t>
+  </si>
+  <si>
+    <t>2864280</t>
+  </si>
+  <si>
+    <t>cardiovascular event</t>
+  </si>
+  <si>
+    <t>107860667</t>
+  </si>
+  <si>
+    <t>4042031</t>
+  </si>
+  <si>
+    <t>bronchial spasm</t>
+  </si>
+  <si>
+    <t>121592367</t>
+  </si>
+  <si>
+    <t>5157652</t>
+  </si>
+  <si>
+    <t>respiratory syncytial virus infections</t>
+  </si>
+  <si>
+    <t>88312302</t>
+  </si>
+  <si>
+    <t>829551</t>
+  </si>
+  <si>
+    <t>hypercapnia</t>
+  </si>
+  <si>
+    <t>98576907</t>
+  </si>
+  <si>
+    <t>3814567</t>
+  </si>
+  <si>
+    <t>silicosis</t>
+  </si>
+  <si>
+    <t>89231438</t>
+  </si>
+  <si>
+    <t>3105217</t>
+  </si>
+  <si>
+    <t>endurance</t>
+  </si>
+  <si>
+    <t>61091155</t>
+  </si>
+  <si>
+    <t>2422249</t>
+  </si>
+  <si>
+    <t>severe asthma</t>
+  </si>
+  <si>
+    <t>77430625</t>
+  </si>
+  <si>
+    <t>2440460</t>
+  </si>
+  <si>
+    <t>severe chronic obstructive pulmonary disease</t>
+  </si>
+  <si>
+    <t>98576922</t>
+  </si>
+  <si>
+    <t>420934</t>
+  </si>
+  <si>
+    <t>paralytic ileus</t>
+  </si>
+  <si>
+    <t>87004859</t>
+  </si>
+  <si>
+    <t>617820</t>
+  </si>
+  <si>
+    <t>smoke inhalation injury</t>
+  </si>
+  <si>
+    <t>112836713</t>
+  </si>
+  <si>
+    <t>3370400</t>
+  </si>
+  <si>
+    <t>disease (or disorder); respiratory tract, acute or subacute, due to chemicals, gases, fumes or vapors (inhalation)</t>
+  </si>
+  <si>
+    <t>115820597</t>
+  </si>
+  <si>
+    <t>777050</t>
+  </si>
+  <si>
+    <t>signal pathways</t>
+  </si>
+  <si>
+    <t>Physiology</t>
+  </si>
+  <si>
+    <t>75971243</t>
+  </si>
+  <si>
+    <t>4041996</t>
+  </si>
+  <si>
+    <t>chemotaxis</t>
+  </si>
+  <si>
+    <t>52932587</t>
+  </si>
+  <si>
+    <t>86265</t>
+  </si>
+  <si>
+    <t>respiratory physiology</t>
+  </si>
+  <si>
+    <t>83642833</t>
+  </si>
+  <si>
+    <t>123514668</t>
+  </si>
+  <si>
+    <t>3257646</t>
+  </si>
+  <si>
+    <t>cytokine biosynthesis</t>
+  </si>
+  <si>
+    <t>82821496</t>
+  </si>
+  <si>
+    <t>78393302</t>
+  </si>
+  <si>
+    <t>3777973</t>
+  </si>
+  <si>
+    <t>pulmonary function</t>
+  </si>
+  <si>
+    <t>96268656</t>
+  </si>
+  <si>
+    <t>309980</t>
+  </si>
+  <si>
+    <t>bronchoconstriction</t>
+  </si>
+  <si>
+    <t>79592456</t>
+  </si>
+  <si>
+    <t>3242189</t>
+  </si>
+  <si>
+    <t>cytokine production</t>
+  </si>
+  <si>
+    <t>82839787</t>
+  </si>
+  <si>
+    <t>3811959</t>
+  </si>
+  <si>
+    <t>neutrophil migration, function</t>
+  </si>
+  <si>
+    <t>68668274</t>
+  </si>
+  <si>
+    <t>4028239</t>
+  </si>
+  <si>
+    <t>mucociliary clearance</t>
+  </si>
+  <si>
+    <t>119598145</t>
+  </si>
+  <si>
+    <t>589077</t>
+  </si>
+  <si>
+    <t>syncytium formation</t>
+  </si>
+  <si>
+    <t>88324477</t>
+  </si>
+  <si>
+    <t>2839339</t>
+  </si>
+  <si>
+    <t>bronchodilation [pe]</t>
+  </si>
+  <si>
+    <t>58238761</t>
   </si>
   <si>
     <t>augments</t>
-  </si>
-  <si>
-    <t>130784477</t>
-  </si>
-  <si>
-    <t>treats</t>
-  </si>
-  <si>
-    <t>344352</t>
-  </si>
-  <si>
-    <t>lung diseases, obstructive</t>
-  </si>
-  <si>
-    <t>159506777</t>
   </si>
 </sst>
 </file>
@@ -445,7 +1138,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5.803170204162598</v>
+        <v>6.502140045166016</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -471,16 +1164,28 @@
       <c r="I2" t="s">
         <v>31</v>
       </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.274158000946045</v>
+        <v>6.2189555168151855</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -495,27 +1200,21 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
       </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.194236755371094</v>
+        <v>5.989805698394775</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -530,27 +1229,21 @@
         <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.084933757781982</v>
+        <v>5.965765953063965</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -565,21 +1258,21 @@
         <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4.0584259033203125</v>
+        <v>5.800235748291016</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -594,21 +1287,21 @@
         <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3.9938769340515137</v>
+        <v>5.765892028808594</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -623,21 +1316,21 @@
         <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3.9434945583343506</v>
+        <v>5.707995891571045</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -652,21 +1345,21 @@
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.717670440673828</v>
+        <v>5.672651767730713</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -681,27 +1374,27 @@
         <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I9" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.602060079574585</v>
+        <v>5.596267223358154</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -716,10 +1409,697 @@
         <v>27</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5.445137023925781</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>5.287801742553711</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5.23223352432251</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>5.201396942138672</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5.185258865356445</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>4.973127841949463</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>4.928907871246338</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>4.893206596374512</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" t="s">
+        <v>90</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>4.757396221160889</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" t="s">
+        <v>94</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>95</v>
+      </c>
+      <c r="M19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>4.71933126449585</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>4.6374897956848145</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" t="s">
+        <v>102</v>
+      </c>
+      <c r="K21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>4.591064453125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>4.469821929931641</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>4.414973258972168</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" t="s">
+        <v>114</v>
+      </c>
+      <c r="J24" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" t="s">
+        <v>116</v>
+      </c>
+      <c r="M24" t="s">
+        <v>117</v>
+      </c>
+      <c r="N24" t="s">
+        <v>118</v>
+      </c>
+      <c r="O24" t="s">
+        <v>42</v>
+      </c>
+      <c r="P24" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>35</v>
+      </c>
+      <c r="R24" t="s">
+        <v>120</v>
+      </c>
+      <c r="S24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>4.0718817710876465</v>
+      </c>
+      <c r="B25" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" t="s">
+        <v>124</v>
+      </c>
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>4.045322895050049</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" t="s">
+        <v>127</v>
+      </c>
+      <c r="I26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" t="s">
+        <v>128</v>
+      </c>
+      <c r="K26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>129</v>
+      </c>
+      <c r="I27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3.949389934539795</v>
+      </c>
+      <c r="B28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" t="s">
+        <v>132</v>
+      </c>
+      <c r="I28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3.748188018798828</v>
+      </c>
+      <c r="B29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" t="s">
+        <v>135</v>
+      </c>
+      <c r="I29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3.602060079574585</v>
+      </c>
+      <c r="B30" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" t="s">
+        <v>138</v>
+      </c>
+      <c r="I30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3.431363821029663</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" t="s">
+        <v>141</v>
+      </c>
+      <c r="I31" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -814,16 +2194,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6.002235412597656</v>
+        <v>6.702395915985107</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -835,24 +2215,30 @@
         <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>146</v>
+      </c>
+      <c r="J2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.537063121795654</v>
+        <v>6.697551727294922</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -864,10 +2250,190 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>6.412393569946289</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>6.097777843475342</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.372543811798096</v>
+      </c>
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5.29203462600708</v>
+      </c>
+      <c r="B7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5.114277362823486</v>
+      </c>
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>167</v>
+      </c>
+      <c r="I8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4.781036853790283</v>
+      </c>
+      <c r="B9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>170</v>
+      </c>
+      <c r="I9" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -962,16 +2528,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4.759214401245117</v>
+        <v>5.744762420654297</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -983,24 +2549,24 @@
         <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.474216461181641</v>
+        <v>5.628490924835205</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -1012,24 +2578,24 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.393399715423584</v>
+        <v>5.2304487228393555</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
@@ -1041,24 +2607,24 @@
         <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>180</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.287353992462158</v>
+        <v>5.173768997192383</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
         <v>28</v>
@@ -1070,24 +2636,24 @@
         <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>183</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.879669189453125</v>
+        <v>5.097257137298584</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>186</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
         <v>28</v>
@@ -1099,10 +2665,39 @@
         <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4.986323833465576</v>
+      </c>
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I7" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1197,16 +2792,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5.299333095550537</v>
+        <v>6.601212501525879</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
         <v>28</v>
@@ -1218,24 +2813,24 @@
         <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
       <c r="I2" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.048985481262207</v>
+        <v>6.250785827636719</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -1247,30 +2842,24 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>198</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
-      </c>
-      <c r="J3" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" t="s">
-        <v>96</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.268578052520752</v>
+        <v>6.2439799308776855</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
@@ -1282,10 +2871,852 @@
         <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>201</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
+        <v>148</v>
+      </c>
+      <c r="J4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>6.221440315246582</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6.155821800231934</v>
+      </c>
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0569047927856445</v>
+      </c>
+      <c r="B7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6.02710485458374</v>
+      </c>
+      <c r="B8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>214</v>
+      </c>
+      <c r="I8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>6.003115653991699</v>
+      </c>
+      <c r="B9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>218</v>
+      </c>
+      <c r="I9" t="s">
+        <v>195</v>
+      </c>
+      <c r="J9" t="s">
+        <v>219</v>
+      </c>
+      <c r="K9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>5.998302936553955</v>
+      </c>
+      <c r="B10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>222</v>
+      </c>
+      <c r="I10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5.790214538574219</v>
+      </c>
+      <c r="B11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>225</v>
+      </c>
+      <c r="I11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>5.751278877258301</v>
+      </c>
+      <c r="B12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" t="s">
+        <v>193</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>228</v>
+      </c>
+      <c r="I12" t="s">
+        <v>229</v>
+      </c>
+      <c r="J12" t="s">
+        <v>230</v>
+      </c>
+      <c r="K12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>5.682506084442139</v>
+      </c>
+      <c r="B13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>233</v>
+      </c>
+      <c r="I13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>5.646991729736328</v>
+      </c>
+      <c r="B14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>237</v>
+      </c>
+      <c r="I14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5.579440593719482</v>
+      </c>
+      <c r="B15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D15" t="s">
+        <v>193</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>240</v>
+      </c>
+      <c r="I15" t="s">
+        <v>195</v>
+      </c>
+      <c r="J15" t="s">
+        <v>241</v>
+      </c>
+      <c r="K15" t="s">
+        <v>184</v>
+      </c>
+      <c r="L15" t="s">
+        <v>242</v>
+      </c>
+      <c r="M15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5.560384750366211</v>
+      </c>
+      <c r="B16" t="s">
+        <v>243</v>
+      </c>
+      <c r="C16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" t="s">
+        <v>245</v>
+      </c>
+      <c r="I16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>5.504062652587891</v>
+      </c>
+      <c r="B17" t="s">
+        <v>246</v>
+      </c>
+      <c r="C17" t="s">
+        <v>247</v>
+      </c>
+      <c r="D17" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>248</v>
+      </c>
+      <c r="I17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>5.503245830535889</v>
+      </c>
+      <c r="B18" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" t="s">
+        <v>193</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
+        <v>251</v>
+      </c>
+      <c r="I18" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>5.472609996795654</v>
+      </c>
+      <c r="B19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D19" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" t="s">
+        <v>254</v>
+      </c>
+      <c r="I19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>5.222456455230713</v>
+      </c>
+      <c r="B20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C20" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>257</v>
+      </c>
+      <c r="I20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>5.122870922088623</v>
+      </c>
+      <c r="B21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" t="s">
+        <v>260</v>
+      </c>
+      <c r="I21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>5.106870651245117</v>
+      </c>
+      <c r="B22" t="s">
+        <v>261</v>
+      </c>
+      <c r="C22" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" t="s">
+        <v>193</v>
+      </c>
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>263</v>
+      </c>
+      <c r="I22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>5.102090358734131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>264</v>
+      </c>
+      <c r="C23" t="s">
+        <v>265</v>
+      </c>
+      <c r="D23" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>266</v>
+      </c>
+      <c r="I23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>5.037824630737305</v>
+      </c>
+      <c r="B24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>4.988112926483154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>270</v>
+      </c>
+      <c r="C25" t="s">
+        <v>271</v>
+      </c>
+      <c r="D25" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s">
+        <v>272</v>
+      </c>
+      <c r="I25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>4.9190778732299805</v>
+      </c>
+      <c r="B26" t="s">
+        <v>273</v>
+      </c>
+      <c r="C26" t="s">
+        <v>274</v>
+      </c>
+      <c r="D26" t="s">
+        <v>193</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" t="s">
+        <v>275</v>
+      </c>
+      <c r="I26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>4.875639915466309</v>
+      </c>
+      <c r="B27" t="s">
+        <v>276</v>
+      </c>
+      <c r="C27" t="s">
+        <v>277</v>
+      </c>
+      <c r="D27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" t="s">
+        <v>278</v>
+      </c>
+      <c r="I27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>4.725911617279053</v>
+      </c>
+      <c r="B28" t="s">
+        <v>279</v>
+      </c>
+      <c r="C28" t="s">
+        <v>280</v>
+      </c>
+      <c r="D28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" t="s">
+        <v>281</v>
+      </c>
+      <c r="I28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>4.659916400909424</v>
+      </c>
+      <c r="B29" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" t="s">
+        <v>283</v>
+      </c>
+      <c r="D29" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" t="s">
+        <v>284</v>
+      </c>
+      <c r="I29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>4.597695350646973</v>
+      </c>
+      <c r="B30" t="s">
+        <v>285</v>
+      </c>
+      <c r="C30" t="s">
+        <v>286</v>
+      </c>
+      <c r="D30" t="s">
+        <v>193</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>27</v>
+      </c>
+      <c r="H30" t="s">
+        <v>287</v>
+      </c>
+      <c r="I30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>4.374748229980469</v>
+      </c>
+      <c r="B31" t="s">
+        <v>288</v>
+      </c>
+      <c r="C31" t="s">
+        <v>289</v>
+      </c>
+      <c r="D31" t="s">
+        <v>193</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" t="s">
+        <v>290</v>
+      </c>
+      <c r="I31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4.3424224853515625</v>
+      </c>
+      <c r="B32" t="s">
+        <v>291</v>
+      </c>
+      <c r="C32" t="s">
+        <v>292</v>
+      </c>
+      <c r="D32" t="s">
+        <v>193</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" t="s">
+        <v>293</v>
+      </c>
+      <c r="I32" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1378,6 +3809,337 @@
         <v>24</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>5.779956817626953</v>
+      </c>
+      <c r="B2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5.68752908706665</v>
+      </c>
+      <c r="B3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>300</v>
+      </c>
+      <c r="I3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5.302114486694336</v>
+      </c>
+      <c r="B4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>303</v>
+      </c>
+      <c r="I4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J4" t="s">
+        <v>304</v>
+      </c>
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5.265289783477783</v>
+      </c>
+      <c r="B5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" t="s">
+        <v>296</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>307</v>
+      </c>
+      <c r="I5" t="s">
+        <v>184</v>
+      </c>
+      <c r="J5" t="s">
+        <v>308</v>
+      </c>
+      <c r="K5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.210586071014404</v>
+      </c>
+      <c r="B6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>311</v>
+      </c>
+      <c r="I6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5.057285785675049</v>
+      </c>
+      <c r="B7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D7" t="s">
+        <v>296</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>314</v>
+      </c>
+      <c r="I7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4.930439472198486</v>
+      </c>
+      <c r="B8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>317</v>
+      </c>
+      <c r="I8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4.913814067840576</v>
+      </c>
+      <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" t="s">
+        <v>296</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>320</v>
+      </c>
+      <c r="I9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4.802089214324951</v>
+      </c>
+      <c r="B10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" t="s">
+        <v>322</v>
+      </c>
+      <c r="D10" t="s">
+        <v>296</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>323</v>
+      </c>
+      <c r="I10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4.653212547302246</v>
+      </c>
+      <c r="B11" t="s">
+        <v>324</v>
+      </c>
+      <c r="C11" t="s">
+        <v>325</v>
+      </c>
+      <c r="D11" t="s">
+        <v>296</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>326</v>
+      </c>
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4.346353054046631</v>
+      </c>
+      <c r="B12" t="s">
+        <v>327</v>
+      </c>
+      <c r="C12" t="s">
+        <v>328</v>
+      </c>
+      <c r="D12" t="s">
+        <v>296</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" t="s">
+        <v>329</v>
+      </c>
+      <c r="I12" t="s">
+        <v>330</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>